<commit_message>
ANOVA pbe résolus, en train de préparer l'affichage des données. Résolu le pbe d'affichage subplot à proportions variables.
</commit_message>
<xml_diff>
--- a/DescData2.1.xlsx
+++ b/DescData2.1.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="420" windowWidth="20115" windowHeight="8520" activeTab="1"/>
+    <workbookView xWindow="1305" yWindow="135" windowWidth="20115" windowHeight="8520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Base de données" sheetId="1" r:id="rId1"/>
     <sheet name="Base de données corrigée" sheetId="4" r:id="rId2"/>
     <sheet name="Indicateurs" sheetId="2" r:id="rId3"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId4"/>
+    <sheet name="topics data_c" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="168">
   <si>
     <t>rows</t>
   </si>
@@ -401,6 +402,126 @@
   </si>
   <si>
     <t>*country_c</t>
+  </si>
+  <si>
+    <t>37 topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Social Protection &amp; Labor: Unemployment'</t>
+  </si>
+  <si>
+    <t>'Secondary'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Primary'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Literacy'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Teachers'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'EMIS'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Attainment'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Education Equality'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Background'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Early Childhood Education'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Tertiary'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Post-Secondary/Non-Tertiary'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Economic Policy &amp; Debt: National accounts: US$ at constant 2010 prices: Aggregate indicators'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Economic Policy &amp; Debt: National accounts: US$ at current prices: Aggregate indicators'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Economic Policy &amp; Debt: Purchasing power parity'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Economic Policy &amp; Debt: National accounts: Atlas GNI &amp; GNI per capita'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Pre-Primary'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Infrastructure: Communications'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Social Protection &amp; Labor: Labor force structure'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Health: Mortality'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Learning Outcomes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Health: Population: Dynamics'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Population'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       'Health: Population: Structure'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Health: Risk factors'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Laber'</t>
+  </si>
+  <si>
+    <t>Expenditures'</t>
+  </si>
+  <si>
+    <t>'Early Child Development (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   'Education Management Information Systems (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   'Engaging the Private Sector (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   'School Autonomy and Accountability (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   'School Finance (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'School Health and School Feeding (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   'Student Assessment (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Teachers (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Tertiary Education (SABER)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Workforce Development (SABER)'</t>
+  </si>
+  <si>
+    <t>Topics de data éliminés dans data_c</t>
+  </si>
+  <si>
+    <t>pas assez données ?</t>
   </si>
 </sst>
 </file>
@@ -738,7 +859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -817,84 +938,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -902,6 +945,93 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1486,79 +1616,79 @@
       <c r="A3" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="65" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="65" t="s">
+      <c r="E3" s="77"/>
+      <c r="F3" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="67"/>
-      <c r="H3" s="65" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="67"/>
-      <c r="J3" s="66" t="s">
+      <c r="I3" s="77"/>
+      <c r="J3" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="K3" s="67"/>
+      <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="63">
+      <c r="B4" s="73">
         <v>886930</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="63">
+      <c r="C4" s="74"/>
+      <c r="D4" s="73">
         <v>241</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="63">
+      <c r="E4" s="78"/>
+      <c r="F4" s="73">
         <v>3665</v>
       </c>
-      <c r="G4" s="68"/>
-      <c r="H4" s="63">
+      <c r="G4" s="78"/>
+      <c r="H4" s="73">
         <v>613</v>
       </c>
-      <c r="I4" s="68"/>
-      <c r="J4" s="64">
+      <c r="I4" s="78"/>
+      <c r="J4" s="74">
         <v>643638</v>
       </c>
-      <c r="K4" s="68"/>
+      <c r="K4" s="78"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="69">
+      <c r="B5" s="79">
         <v>69</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="69">
+      <c r="C5" s="80"/>
+      <c r="D5" s="79">
         <v>31</v>
       </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="69">
+      <c r="E5" s="80"/>
+      <c r="F5" s="79">
         <v>20</v>
       </c>
-      <c r="G5" s="70"/>
-      <c r="H5" s="69">
+      <c r="G5" s="80"/>
+      <c r="H5" s="79">
         <v>3</v>
       </c>
-      <c r="I5" s="70"/>
-      <c r="J5" s="69">
+      <c r="I5" s="80"/>
+      <c r="J5" s="79">
         <v>4</v>
       </c>
-      <c r="K5" s="70"/>
+      <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="51" t="s">
         <v>101</v>
       </c>
@@ -1591,7 +1721,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="51" t="s">
         <v>55</v>
       </c>
@@ -1624,7 +1754,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="51" t="s">
         <v>57</v>
       </c>
@@ -1657,7 +1787,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
+      <c r="A9" s="71"/>
       <c r="B9" s="51" t="s">
         <v>56</v>
       </c>
@@ -1686,7 +1816,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="51" t="s">
         <v>4</v>
       </c>
@@ -1709,7 +1839,7 @@
       <c r="K10" s="53"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="33" t="s">
         <v>3</v>
       </c>
@@ -1732,7 +1862,7 @@
       <c r="K11" s="34"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="33"/>
       <c r="C12" s="50"/>
       <c r="D12" s="33" t="s">
@@ -1753,7 +1883,7 @@
       <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="33"/>
       <c r="C13" s="50"/>
       <c r="D13" s="33" t="s">
@@ -1774,7 +1904,7 @@
       <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="33"/>
       <c r="C14" s="50"/>
       <c r="D14" s="33" t="s">
@@ -1795,7 +1925,7 @@
       <c r="K14" s="34"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="33"/>
       <c r="C15" s="50"/>
       <c r="D15" s="33" t="s">
@@ -1816,7 +1946,7 @@
       <c r="K15" s="34"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="33"/>
       <c r="C16" s="50"/>
       <c r="D16" s="33" t="s">
@@ -1837,7 +1967,7 @@
       <c r="K16" s="34"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
+      <c r="A17" s="71"/>
       <c r="B17" s="33"/>
       <c r="C17" s="50"/>
       <c r="D17" s="33" t="s">
@@ -1858,7 +1988,7 @@
       <c r="K17" s="34"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
+      <c r="A18" s="71"/>
       <c r="B18" s="33"/>
       <c r="C18" s="50"/>
       <c r="D18" s="33" t="s">
@@ -1879,7 +2009,7 @@
       <c r="K18" s="34"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="33"/>
       <c r="C19" s="50"/>
       <c r="D19" s="33" t="s">
@@ -1900,7 +2030,7 @@
       <c r="K19" s="34"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="33"/>
       <c r="C20" s="50"/>
       <c r="D20" s="33" t="s">
@@ -1921,7 +2051,7 @@
       <c r="K20" s="34"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="61"/>
+      <c r="A21" s="71"/>
       <c r="B21" s="33"/>
       <c r="C21" s="50"/>
       <c r="D21" s="33" t="s">
@@ -1942,7 +2072,7 @@
       <c r="K21" s="34"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="61"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="33"/>
       <c r="C22" s="50"/>
       <c r="D22" s="33" t="s">
@@ -1963,7 +2093,7 @@
       <c r="K22" s="34"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="61"/>
+      <c r="A23" s="71"/>
       <c r="B23" s="33"/>
       <c r="C23" s="50"/>
       <c r="D23" s="33" t="s">
@@ -1984,7 +2114,7 @@
       <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
+      <c r="A24" s="71"/>
       <c r="B24" s="33"/>
       <c r="C24" s="50"/>
       <c r="D24" s="33" t="s">
@@ -2005,7 +2135,7 @@
       <c r="K24" s="34"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
+      <c r="A25" s="71"/>
       <c r="B25" s="33"/>
       <c r="C25" s="50"/>
       <c r="D25" s="33" t="s">
@@ -2026,7 +2156,7 @@
       <c r="K25" s="34"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="33"/>
       <c r="C26" s="50"/>
       <c r="D26" s="33" t="s">
@@ -2043,7 +2173,7 @@
       <c r="K26" s="34"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
+      <c r="A27" s="71"/>
       <c r="B27" s="33"/>
       <c r="C27" s="50"/>
       <c r="D27" s="33" t="s">
@@ -2060,7 +2190,7 @@
       <c r="K27" s="34"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="33"/>
       <c r="C28" s="50"/>
       <c r="D28" s="33" t="s">
@@ -2077,7 +2207,7 @@
       <c r="K28" s="34"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="33"/>
       <c r="C29" s="50"/>
       <c r="D29" s="33" t="s">
@@ -2094,7 +2224,7 @@
       <c r="K29" s="34"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="33"/>
       <c r="C30" s="50"/>
       <c r="D30" s="33" t="s">
@@ -2111,7 +2241,7 @@
       <c r="K30" s="34"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
+      <c r="A31" s="71"/>
       <c r="B31" s="33"/>
       <c r="C31" s="50"/>
       <c r="D31" s="33" t="s">
@@ -2128,7 +2258,7 @@
       <c r="K31" s="34"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="33"/>
       <c r="C32" s="50"/>
       <c r="D32" s="33" t="s">
@@ -2145,7 +2275,7 @@
       <c r="K32" s="34"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="61"/>
+      <c r="A33" s="71"/>
       <c r="B33" s="33"/>
       <c r="C33" s="50"/>
       <c r="D33" s="33" t="s">
@@ -2162,7 +2292,7 @@
       <c r="K33" s="34"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="61"/>
+      <c r="A34" s="71"/>
       <c r="B34" s="33"/>
       <c r="C34" s="50"/>
       <c r="D34" s="33" t="s">
@@ -2179,7 +2309,7 @@
       <c r="K34" s="34"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="61"/>
+      <c r="A35" s="71"/>
       <c r="B35" s="33"/>
       <c r="C35" s="50"/>
       <c r="D35" s="33" t="s">
@@ -2196,7 +2326,7 @@
       <c r="K35" s="34"/>
     </row>
     <row r="36" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="62"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="55"/>
       <c r="C36" s="56"/>
       <c r="D36" s="55" t="s">
@@ -2303,7 +2433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2351,116 +2481,116 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="61" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="93" t="s">
+      <c r="C5" s="97"/>
+      <c r="D5" s="98" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="94"/>
-      <c r="F5" s="95" t="s">
+      <c r="E5" s="99"/>
+      <c r="F5" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="G5" s="96"/>
-      <c r="H5" s="97" t="s">
+      <c r="G5" s="101"/>
+      <c r="H5" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="98"/>
-      <c r="J5" s="99" t="s">
+      <c r="I5" s="103"/>
+      <c r="J5" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="K5" s="100"/>
+      <c r="K5" s="105"/>
     </row>
     <row r="6" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="75" t="s">
+      <c r="C6" s="84"/>
+      <c r="D6" s="85" t="s">
         <v>127</v>
       </c>
-      <c r="E6" s="76"/>
-      <c r="F6" s="77" t="s">
+      <c r="E6" s="86"/>
+      <c r="F6" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="78"/>
-      <c r="H6" s="79" t="s">
+      <c r="G6" s="88"/>
+      <c r="H6" s="89" t="s">
         <v>118</v>
       </c>
-      <c r="I6" s="80"/>
-      <c r="J6" s="81" t="s">
+      <c r="I6" s="90"/>
+      <c r="J6" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="K6" s="82"/>
+      <c r="K6" s="92"/>
     </row>
     <row r="7" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="83">
+      <c r="B7" s="93">
         <v>886930</v>
       </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="83">
+      <c r="C7" s="94"/>
+      <c r="D7" s="93">
         <v>242</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="83">
+      <c r="E7" s="95"/>
+      <c r="F7" s="93">
         <v>3665</v>
       </c>
-      <c r="G7" s="85"/>
-      <c r="H7" s="83">
+      <c r="G7" s="95"/>
+      <c r="H7" s="93">
         <v>613</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="84">
+      <c r="I7" s="95"/>
+      <c r="J7" s="94">
         <v>643638</v>
       </c>
-      <c r="K7" s="85"/>
+      <c r="K7" s="95"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="71">
+      <c r="B8" s="81">
         <v>69</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="71">
+      <c r="C8" s="82"/>
+      <c r="D8" s="81">
         <v>31</v>
       </c>
-      <c r="E8" s="72"/>
-      <c r="F8" s="71">
+      <c r="E8" s="82"/>
+      <c r="F8" s="81">
         <v>20</v>
       </c>
-      <c r="G8" s="72"/>
-      <c r="H8" s="71">
+      <c r="G8" s="82"/>
+      <c r="H8" s="81">
         <v>3</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="71">
+      <c r="I8" s="82"/>
+      <c r="J8" s="81">
         <v>4</v>
       </c>
-      <c r="K8" s="72"/>
+      <c r="K8" s="82"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
-      <c r="B9" s="89" t="s">
+      <c r="A9" s="71"/>
+      <c r="B9" s="63" t="s">
         <v>101</v>
       </c>
       <c r="C9" s="29">
@@ -2492,7 +2622,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="7" t="s">
         <v>55</v>
       </c>
@@ -2525,8 +2655,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
-      <c r="B11" s="90" t="s">
+      <c r="A11" s="71"/>
+      <c r="B11" s="64" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="43">
@@ -2538,7 +2668,7 @@
       <c r="E11" s="14">
         <v>242</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="62" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="39">
@@ -2558,7 +2688,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="44" t="s">
         <v>56</v>
       </c>
@@ -2587,7 +2717,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
@@ -2610,7 +2740,7 @@
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="8" t="s">
         <v>3</v>
       </c>
@@ -2633,7 +2763,7 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="5"/>
       <c r="C15" s="17"/>
       <c r="D15" s="6" t="s">
@@ -2654,7 +2784,7 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="5"/>
       <c r="C16" s="17"/>
       <c r="D16" s="6" t="s">
@@ -2675,7 +2805,7 @@
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
+      <c r="A17" s="71"/>
       <c r="B17" s="5"/>
       <c r="C17" s="17"/>
       <c r="D17" s="6" t="s">
@@ -2696,7 +2826,7 @@
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
+      <c r="A18" s="71"/>
       <c r="B18" s="5"/>
       <c r="C18" s="17"/>
       <c r="D18" s="6" t="s">
@@ -2717,7 +2847,7 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="5"/>
       <c r="C19" s="17"/>
       <c r="D19" s="6" t="s">
@@ -2738,7 +2868,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="5"/>
       <c r="C20" s="17"/>
       <c r="D20" s="6" t="s">
@@ -2759,7 +2889,7 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="61"/>
+      <c r="A21" s="71"/>
       <c r="B21" s="5"/>
       <c r="C21" s="17"/>
       <c r="D21" s="6" t="s">
@@ -2780,7 +2910,7 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="61"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="5"/>
       <c r="C22" s="17"/>
       <c r="D22" s="6" t="s">
@@ -2801,7 +2931,7 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="61"/>
+      <c r="A23" s="71"/>
       <c r="B23" s="5"/>
       <c r="C23" s="17"/>
       <c r="D23" s="6" t="s">
@@ -2822,7 +2952,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
+      <c r="A24" s="71"/>
       <c r="B24" s="5"/>
       <c r="C24" s="17"/>
       <c r="D24" s="6" t="s">
@@ -2843,7 +2973,7 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
+      <c r="A25" s="71"/>
       <c r="B25" s="5"/>
       <c r="C25" s="17"/>
       <c r="D25" s="6" t="s">
@@ -2864,7 +2994,7 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="5"/>
       <c r="C26" s="17"/>
       <c r="D26" s="6" t="s">
@@ -2885,7 +3015,7 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
+      <c r="A27" s="71"/>
       <c r="B27" s="5"/>
       <c r="C27" s="17"/>
       <c r="D27" s="6" t="s">
@@ -2906,7 +3036,7 @@
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="5"/>
       <c r="C28" s="17"/>
       <c r="D28" s="6" t="s">
@@ -2927,7 +3057,7 @@
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="5"/>
       <c r="C29" s="17"/>
       <c r="D29" s="6" t="s">
@@ -2944,7 +3074,7 @@
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="5"/>
       <c r="C30" s="17"/>
       <c r="D30" s="6" t="s">
@@ -2961,7 +3091,7 @@
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
+      <c r="A31" s="71"/>
       <c r="B31" s="5"/>
       <c r="C31" s="17"/>
       <c r="D31" s="6" t="s">
@@ -2978,7 +3108,7 @@
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="5"/>
       <c r="C32" s="17"/>
       <c r="D32" s="6" t="s">
@@ -2995,7 +3125,7 @@
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="61"/>
+      <c r="A33" s="71"/>
       <c r="B33" s="5"/>
       <c r="C33" s="17"/>
       <c r="D33" s="6" t="s">
@@ -3012,7 +3142,7 @@
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="61"/>
+      <c r="A34" s="71"/>
       <c r="B34" s="5"/>
       <c r="C34" s="17"/>
       <c r="D34" s="6" t="s">
@@ -3029,7 +3159,7 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="61"/>
+      <c r="A35" s="71"/>
       <c r="B35" s="5"/>
       <c r="C35" s="17"/>
       <c r="D35" s="6" t="s">
@@ -3046,7 +3176,7 @@
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36" s="61"/>
+      <c r="A36" s="71"/>
       <c r="B36" s="5"/>
       <c r="C36" s="17"/>
       <c r="D36" s="6" t="s">
@@ -3063,7 +3193,7 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A37" s="61"/>
+      <c r="A37" s="71"/>
       <c r="B37" s="5"/>
       <c r="C37" s="17"/>
       <c r="D37" s="6" t="s">
@@ -3080,7 +3210,7 @@
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38" s="61"/>
+      <c r="A38" s="71"/>
       <c r="B38" s="5"/>
       <c r="C38" s="17"/>
       <c r="D38" s="6" t="s">
@@ -3097,7 +3227,7 @@
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="62"/>
+      <c r="A39" s="72"/>
       <c r="B39" s="9"/>
       <c r="C39" s="18"/>
       <c r="D39" s="41" t="s">
@@ -3210,7 +3340,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3363,6 +3493,9 @@
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>82</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -3396,16 +3529,100 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D11:L17"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="C4:N21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="88.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D11" s="21"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" t="s">
+        <v>162</v>
+      </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
@@ -3414,23 +3631,97 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="21"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="65" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="65" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="65" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="65" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="65" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="67" t="s">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Avant RV mentor num 4.
</commit_message>
<xml_diff>
--- a/DescData2.1.xlsx
+++ b/DescData2.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="185">
   <si>
     <t>rows</t>
   </si>
@@ -522,6 +522,57 @@
   </si>
   <si>
     <t>pas assez données ?</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>SABER</t>
   </si>
 </sst>
 </file>
@@ -859,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1062,6 +1113,8 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3529,198 +3582,259 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="88.140625" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="64" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
+        <v>168</v>
+      </c>
       <c r="B1" s="65" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="65" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="68" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="69" t="s">
+      <c r="C3" s="65" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="69" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="65" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="106" t="s">
+        <v>171</v>
+      </c>
       <c r="B4" s="66" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="66" t="s">
+      <c r="C4" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="106" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="106" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="106" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="106" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="106"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="106"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="106" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="106" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="106" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="106" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="106"/>
+      <c r="B17" s="107"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="106"/>
+      <c r="B18" s="107"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="106" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="106" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" s="107" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="66" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>14</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" t="s">
-        <v>162</v>
-      </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="66" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="66" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="65" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="65" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="65" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="65" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="65" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="65" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="65" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="65" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="65" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="65" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="65" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="67" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>